<commit_message>
question data changes changes
</commit_message>
<xml_diff>
--- a/lib/questions.xlsx
+++ b/lib/questions.xlsx
@@ -217,7 +217,7 @@
     <t>When they heard news of the hurricane, Maya and Julian decided to change their vacation plans. Instead of traveling to the island beach resort, they booked a room at a fancy new spa in the mountains. Their plans were a bit more expensive, but they'd heard wonderful things about the spa and they were relieved to find availability on such short notice.</t>
   </si>
   <si>
-    <t>["Maya and Julian take beach vacations every year.", "The spa is overpriced." "It is usually necessary to book at least six months in advance at the spa.", "Maya and Julian decided to change their vacation plans because of the hurricane."]</t>
+    <t>["Maya and Julian take beach vacations every year.", "The spa is overpriced.", "It is usually necessary to book at least six months in advance at the spa.", "Maya and Julian decided to change their vacation plans because of the hurricane."]</t>
   </si>
   <si>
     <t>Maya and Julian decided to change their vacation plans because of the hurricane.</t>
@@ -284,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -311,6 +311,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1286,7 +1289,7 @@
       <c r="C21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="9" t="s">
         <v>68</v>
       </c>
       <c r="E21" s="4" t="s">

</xml_diff>